<commit_message>
Commiting the presentation deck
</commit_message>
<xml_diff>
--- a/Forecast checks_23 Apr.xlsx
+++ b/Forecast checks_23 Apr.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akhilajoseph/Documents/DS/Projects/Akhila-Joseph-Projects/Project_5/Covid-19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B509A6-939E-9342-8695-E427DA8B5D37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2180B0-4E2A-5747-AEBD-5A5117EEA344}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13120" yWindow="-16460" windowWidth="18660" windowHeight="13420" activeTab="3" xr2:uid="{33AF708B-0BA3-1049-82BF-C130CD4F8AE1}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" activeTab="4" xr2:uid="{33AF708B-0BA3-1049-82BF-C130CD4F8AE1}"/>
   </bookViews>
   <sheets>
     <sheet name="5 steps" sheetId="11" r:id="rId1"/>
     <sheet name="6 steps" sheetId="8" r:id="rId2"/>
     <sheet name="7 steps" sheetId="9" r:id="rId3"/>
     <sheet name="3 steps" sheetId="10" r:id="rId4"/>
+    <sheet name="5 steps_24 Apr" sheetId="12" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="8">
   <si>
     <t>confirmed</t>
   </si>
@@ -58,12 +59,15 @@
   <si>
     <t>F MAPE</t>
   </si>
+  <si>
+    <t xml:space="preserve">Avg MAPE: </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -106,8 +110,61 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -117,6 +174,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -134,7 +203,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -157,6 +226,34 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="11" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="12" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,7 +572,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView zoomScale="144" zoomScaleNormal="144" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12:G15"/>
+      <selection activeCell="D12" sqref="D12:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1779,7 +1876,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D83ECF0-E347-A84D-9CC9-38D2AB89E56B}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="144" zoomScaleNormal="144" workbookViewId="0">
+    <sheetView zoomScale="144" zoomScaleNormal="144" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -2208,4 +2305,451 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8F2766B-336E-8D45-95FA-8625AF6599D8}">
+  <dimension ref="A2:H24"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="6.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="6.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B2" s="18"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="25">
+        <f>AVERAGE(G4:G16)</f>
+        <v>3.9961021018314884E-2</v>
+      </c>
+      <c r="H2" s="25">
+        <f>AVERAGE(H4:H16)</f>
+        <v>3.8874238360868611E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B3" s="18"/>
+      <c r="C3" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B4" s="16">
+        <v>43931</v>
+      </c>
+      <c r="C4" s="14">
+        <v>1657526</v>
+      </c>
+      <c r="D4" s="15">
+        <v>1576827</v>
+      </c>
+      <c r="E4" s="14">
+        <v>102525</v>
+      </c>
+      <c r="F4" s="15">
+        <v>98456</v>
+      </c>
+      <c r="G4" s="17">
+        <f>ABS((C4-D4))/C4</f>
+        <v>4.8686415778696687E-2</v>
+      </c>
+      <c r="H4" s="17">
+        <f>ABS((E4-F4))/E4</f>
+        <v>3.9687881004633017E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B5" s="16">
+        <v>43932</v>
+      </c>
+      <c r="C5" s="14">
+        <v>1735650</v>
+      </c>
+      <c r="D5" s="15">
+        <v>1657472</v>
+      </c>
+      <c r="E5" s="14">
+        <v>108502</v>
+      </c>
+      <c r="F5" s="15">
+        <v>104154</v>
+      </c>
+      <c r="G5" s="17">
+        <f t="shared" ref="G5:G16" si="0">ABS((C5-D5))/C5</f>
+        <v>4.5042491285685479E-2</v>
+      </c>
+      <c r="H5" s="17">
+        <f t="shared" ref="H5:H16" si="1">ABS((E5-F5))/E5</f>
+        <v>4.0072994046192696E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B6" s="16">
+        <v>43933</v>
+      </c>
+      <c r="C6" s="14">
+        <v>1834721</v>
+      </c>
+      <c r="D6" s="15">
+        <v>1741973</v>
+      </c>
+      <c r="E6" s="14">
+        <v>114090</v>
+      </c>
+      <c r="F6" s="15">
+        <v>110201</v>
+      </c>
+      <c r="G6" s="17">
+        <f t="shared" si="0"/>
+        <v>5.0551555250089794E-2</v>
+      </c>
+      <c r="H6" s="17">
+        <f t="shared" si="1"/>
+        <v>3.4087124200192831E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="16">
+        <v>43934</v>
+      </c>
+      <c r="C7" s="14">
+        <v>1904838</v>
+      </c>
+      <c r="D7" s="15">
+        <v>1826314</v>
+      </c>
+      <c r="E7" s="14">
+        <v>119481</v>
+      </c>
+      <c r="F7" s="15">
+        <v>116253</v>
+      </c>
+      <c r="G7" s="17">
+        <f t="shared" si="0"/>
+        <v>4.1223453123047732E-2</v>
+      </c>
+      <c r="H7" s="17">
+        <f t="shared" si="1"/>
+        <v>2.7016847867024883E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="16">
+        <v>43935</v>
+      </c>
+      <c r="C8" s="14">
+        <v>1976191</v>
+      </c>
+      <c r="D8" s="15">
+        <v>1911048</v>
+      </c>
+      <c r="E8" s="14">
+        <v>125983</v>
+      </c>
+      <c r="F8" s="15">
+        <v>122352</v>
+      </c>
+      <c r="G8" s="17">
+        <f t="shared" si="0"/>
+        <v>3.2963918973419069E-2</v>
+      </c>
+      <c r="H8" s="17">
+        <f t="shared" si="1"/>
+        <v>2.8821348912154814E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="16">
+        <v>43936</v>
+      </c>
+      <c r="C9" s="14">
+        <v>2056054</v>
+      </c>
+      <c r="D9" s="15">
+        <v>1995154</v>
+      </c>
+      <c r="E9" s="14">
+        <v>134176</v>
+      </c>
+      <c r="F9" s="15">
+        <v>128423</v>
+      </c>
+      <c r="G9" s="17">
+        <f t="shared" si="0"/>
+        <v>2.9619844614976066E-2</v>
+      </c>
+      <c r="H9" s="17">
+        <f t="shared" si="1"/>
+        <v>4.2876520391128069E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="16">
+        <v>43937</v>
+      </c>
+      <c r="C10" s="14">
+        <v>2152437</v>
+      </c>
+      <c r="D10" s="15">
+        <v>2095004</v>
+      </c>
+      <c r="E10" s="14">
+        <v>143800</v>
+      </c>
+      <c r="F10" s="15">
+        <v>135609</v>
+      </c>
+      <c r="G10" s="17">
+        <f t="shared" si="0"/>
+        <v>2.6682778636494354E-2</v>
+      </c>
+      <c r="H10" s="17">
+        <f t="shared" si="1"/>
+        <v>5.696105702364395E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="16">
+        <v>43938</v>
+      </c>
+      <c r="C11" s="14">
+        <v>2240190</v>
+      </c>
+      <c r="D11" s="15">
+        <v>2200968</v>
+      </c>
+      <c r="E11" s="14">
+        <v>153821</v>
+      </c>
+      <c r="F11" s="15">
+        <v>143299</v>
+      </c>
+      <c r="G11" s="17">
+        <f t="shared" si="0"/>
+        <v>1.7508336346470612E-2</v>
+      </c>
+      <c r="H11" s="17">
+        <f t="shared" si="1"/>
+        <v>6.8404184084097749E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="16">
+        <v>43939</v>
+      </c>
+      <c r="C12" s="14">
+        <v>2317758</v>
+      </c>
+      <c r="D12" s="15">
+        <v>2314051</v>
+      </c>
+      <c r="E12" s="14">
+        <v>159509</v>
+      </c>
+      <c r="F12" s="15">
+        <v>151536</v>
+      </c>
+      <c r="G12" s="17">
+        <f t="shared" si="0"/>
+        <v>1.5993904454218257E-3</v>
+      </c>
+      <c r="H12" s="17">
+        <f t="shared" si="1"/>
+        <v>4.9984640365120465E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="21">
+        <v>43940</v>
+      </c>
+      <c r="C13" s="22">
+        <v>2401101</v>
+      </c>
+      <c r="D13" s="23">
+        <v>2436595</v>
+      </c>
+      <c r="E13" s="22">
+        <v>165043</v>
+      </c>
+      <c r="F13" s="23">
+        <v>160489</v>
+      </c>
+      <c r="G13" s="24">
+        <f t="shared" si="0"/>
+        <v>1.4782385247434407E-2</v>
+      </c>
+      <c r="H13" s="24">
+        <f t="shared" si="1"/>
+        <v>2.7592809146707222E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="21">
+        <v>43941</v>
+      </c>
+      <c r="C14" s="22">
+        <v>2472258</v>
+      </c>
+      <c r="D14" s="23">
+        <v>2571556</v>
+      </c>
+      <c r="E14" s="22">
+        <v>169985</v>
+      </c>
+      <c r="F14" s="23">
+        <v>170368</v>
+      </c>
+      <c r="G14" s="24">
+        <f t="shared" si="0"/>
+        <v>4.0164901883217689E-2</v>
+      </c>
+      <c r="H14" s="24">
+        <f t="shared" si="1"/>
+        <v>2.253139982939671E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="21">
+        <v>43942</v>
+      </c>
+      <c r="C15" s="22">
+        <v>2549293</v>
+      </c>
+      <c r="D15" s="23">
+        <v>2723091</v>
+      </c>
+      <c r="E15" s="22">
+        <v>176582</v>
+      </c>
+      <c r="F15" s="23">
+        <v>181493</v>
+      </c>
+      <c r="G15" s="24">
+        <f t="shared" si="0"/>
+        <v>6.8174980278845942E-2</v>
+      </c>
+      <c r="H15" s="24">
+        <f t="shared" si="1"/>
+        <v>2.7811441709800547E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="21">
+        <v>43943</v>
+      </c>
+      <c r="C16" s="22">
+        <v>2623413</v>
+      </c>
+      <c r="D16" s="23">
+        <v>2892294</v>
+      </c>
+      <c r="E16" s="22">
+        <v>183025</v>
+      </c>
+      <c r="F16" s="23">
+        <v>193969</v>
+      </c>
+      <c r="G16" s="24">
+        <f t="shared" si="0"/>
+        <v>0.10249282137429372</v>
+      </c>
+      <c r="H16" s="24">
+        <f t="shared" si="1"/>
+        <v>5.9795109957656058E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" s="16">
+        <v>43944</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="15">
+        <v>3083536</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" s="15">
+        <v>208135</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" s="16">
+        <v>43945</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="15">
+        <v>3303240</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="15">
+        <v>224424</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" s="16">
+        <v>43946</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="15">
+        <v>3559400</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" s="15">
+        <v>243438</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E24" s="13">
+        <v>176582</v>
+      </c>
+      <c r="F24" s="12">
+        <v>183025</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>